<commit_message>
added chatGPT prompt engineering for developers
</commit_message>
<xml_diff>
--- a/data/prompt_engineering.xlsx
+++ b/data/prompt_engineering.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tcs\chatGPT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0322DDCF-A1D8-4CE1-AE21-ABEAB04285B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE524AF2-AF63-415B-8695-222B8D63ECBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="4550" windowWidth="21710" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27180" yWindow="4550" windowWidth="21710" windowHeight="12240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guidelines" sheetId="1" r:id="rId1"/>
+    <sheet name="---" sheetId="3" r:id="rId2"/>
+    <sheet name="summary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>원칙</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +66,94 @@
   </si>
   <si>
     <t>세부책략</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간략한 요약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(배송/배달/가격) 초점 두고 요약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요약 대신 관련부문 추출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(긍/부정) 감성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감정 유형 식별</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객 분노 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제품과 회사명 추출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한번에 반복작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토필 추론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>번역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>언어감지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>격시 및 비격식 문장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범용 글로벌 번역기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료형(JSON 등) 변환</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문법/맞춤법 교정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세부작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>챗봇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실무작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어조 변환</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -107,8 +197,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -391,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -462,4 +555,190 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBBB914-F931-43C2-9781-21327B33AA09}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EC647-B1A1-4394-92CE-59304463E1A6}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>